<commit_message>
25 fruit icon added
</commit_message>
<xml_diff>
--- a/Pre-GDC-prototype-addiction/Assets/Art/GDCprototypeGDD.xlsx
+++ b/Pre-GDC-prototype-addiction/Assets/Art/GDCprototypeGDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Pre-GDC\Pre-GDC-prototype-addiction\Assets\Art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C22D7D71-DF50-43D6-B1DC-C8E7BD784973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4A1DAF-1C29-49BC-909F-44221634E7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E76E6AB4-BD6D-4614-9422-5480CEB87A36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{E76E6AB4-BD6D-4614-9422-5480CEB87A36}"/>
   </bookViews>
   <sheets>
     <sheet name="pre-gdc prototype" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Pre-GDC Prototype design doc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,6 +186,10 @@
   </si>
   <si>
     <t>玻璃板子？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>card check</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -274,9 +278,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -288,6 +289,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1805,15 +1809,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1828,7 +1832,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4400550" y="1400175"/>
+          <a:off x="4324350" y="1590675"/>
           <a:ext cx="5886450" cy="4629150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2711,18 +2715,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A79569-AB25-4370-90C4-15D0D44E0596}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" s="5" customFormat="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="1" customFormat="1"/>
+    <row r="2" spans="1:1" s="5" customFormat="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:XFD2"/>
@@ -2734,47 +2738,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294394B7-76CC-4476-B2B9-EAC2F8A3415D}">
-  <dimension ref="A1:X208"/>
+  <dimension ref="A1:Z208"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P205" sqref="P205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" s="5" customFormat="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="1" customFormat="1"/>
-    <row r="4" spans="1:24">
-      <c r="A4" s="3" t="s">
+    <row r="2" spans="1:26" s="5" customFormat="1"/>
+    <row r="4" spans="1:26">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="15" spans="1:24">
-      <c r="X15" t="s">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="Z14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="24:24">
-      <c r="X17" t="s">
+    <row r="16" spans="1:26">
+      <c r="Z16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="1"/>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C49" s="4"/>
+      <c r="C49" s="3"/>
     </row>
     <row r="51" spans="2:4">
       <c r="D51" t="s">
@@ -2787,12 +2791,12 @@
       </c>
     </row>
     <row r="73" spans="2:4">
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="75" spans="2:4">
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2807,7 +2811,7 @@
       </c>
     </row>
     <row r="95" spans="3:3">
-      <c r="C95" s="5" t="s">
+      <c r="C95" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2817,7 +2821,7 @@
       </c>
     </row>
     <row r="99" spans="3:4">
-      <c r="C99" s="5" t="s">
+      <c r="C99" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2837,7 +2841,7 @@
       </c>
     </row>
     <row r="126" spans="3:4">
-      <c r="C126" s="5" t="s">
+      <c r="C126" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2846,27 +2850,42 @@
         <v>35</v>
       </c>
     </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="B132" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="B138" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="149" spans="1:2">
-      <c r="A149" s="3" t="s">
+      <c r="A149" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B149" s="2"/>
+      <c r="B149" s="1"/>
     </row>
     <row r="151" spans="1:2">
-      <c r="B151" s="4" t="s">
+      <c r="B151" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="176" spans="2:2">
-      <c r="B176" s="4" t="s">
+      <c r="B176" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="203" spans="1:3">
-      <c r="B203" s="4" t="s">
+      <c r="B203" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C203" s="4"/>
+      <c r="C203" s="3"/>
     </row>
     <row r="205" spans="1:3">
       <c r="C205" t="s">
@@ -2874,8 +2893,8 @@
       </c>
     </row>
     <row r="208" spans="1:3">
-      <c r="A208" s="3"/>
-      <c r="B208" s="2"/>
+      <c r="A208" s="2"/>
+      <c r="B208" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2897,24 +2916,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" s="5" customFormat="1">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="1" customFormat="1"/>
+    <row r="2" spans="1:1" s="5" customFormat="1"/>
     <row r="4" spans="1:1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2932,53 +2951,53 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" s="5" customFormat="1">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1"/>
+    <row r="2" spans="1:2" s="5" customFormat="1"/>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="2"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>